<commit_message>
Placed LEDs with 1:60 scale
</commit_message>
<xml_diff>
--- a/uka17.xlsx
+++ b/uka17.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Mikrolysreklamen17\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="uka15" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -39,8 +34,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,48 +517,48 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Inndata" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Koblet celle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Kontrollcelle" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Merknad" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Nøytral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Tittel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totalt" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -621,7 +616,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -656,7 +651,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -833,26 +828,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1">
         <v>1</v>
       </c>
@@ -864,28 +859,28 @@
       </c>
       <c r="F1" s="1">
         <f>(B1*1000)/$M$1</f>
-        <v>6.8</v>
+        <v>4.25</v>
       </c>
       <c r="G1" s="1">
         <f>(C1*1000)/$M$1</f>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="I1">
-        <f>(F1+$M$4)*$M$2</f>
-        <v>29.3</v>
+        <f>(F1*$M$2)+$M$4</f>
+        <v>26.75</v>
       </c>
       <c r="J1">
-        <f>(G1+$M$5)*$M$3</f>
-        <v>6</v>
+        <f>(G1*$M$3)+$M$5</f>
+        <v>3.75</v>
       </c>
       <c r="L1" t="s">
         <v>0</v>
       </c>
       <c r="M1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>2</v>
       </c>
@@ -897,19 +892,19 @@
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F65" si="0">(B2*1000)/$M$1</f>
-        <v>8.8000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G65" si="1">(C2*1000)/$M$1</f>
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I65" si="2">(F2+$M$4)*$M$2</f>
-        <v>31.3</v>
+        <f t="shared" ref="I2:I65" si="2">(F2*$M$2)+$M$4</f>
+        <v>28</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J65" si="3">(G2+$M$5)*$M$3</f>
-        <v>12</v>
+        <f t="shared" ref="J2:J65" si="3">(G2*$M$3)+$M$5</f>
+        <v>7.5</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
@@ -918,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>3</v>
       </c>
@@ -930,19 +925,19 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>6.8</v>
+        <v>4.25</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>11.25</v>
       </c>
       <c r="I3">
         <f t="shared" si="2"/>
-        <v>29.3</v>
+        <v>26.75</v>
       </c>
       <c r="J3">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>11.25</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
@@ -951,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>4</v>
       </c>
@@ -963,19 +958,19 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>31.3</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
@@ -984,7 +979,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>5</v>
       </c>
@@ -996,19 +991,19 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>6.8</v>
+        <v>4.25</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>18.75</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>29.3</v>
+        <v>26.75</v>
       </c>
       <c r="J5">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>18.75</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -1017,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1029,22 +1024,22 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>22.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>31.3</v>
+        <v>28</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1056,22 +1051,22 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>1.75</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>32.4</v>
+        <v>20.25</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>25.3</v>
+        <v>24.25</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>32.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1083,22 +1078,22 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>6.25</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>35.299999999999997</v>
+        <v>30.5</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1110,22 +1105,22 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>17.600000000000001</v>
+        <v>11</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>35.299999999999997</v>
+        <v>30.5</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>17.600000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1137,22 +1132,22 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>25.2</v>
+        <v>15.75</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>35.299999999999997</v>
+        <v>30.5</v>
       </c>
       <c r="J10">
         <f t="shared" si="3"/>
-        <v>25.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1164,22 +1159,22 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>32.799999999999997</v>
+        <v>20.5</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>35.299999999999997</v>
+        <v>30.5</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1191,22 +1186,22 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>13.8</v>
+        <v>8.625</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>40.799999999999997</v>
+        <v>25.5</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>36.299999999999997</v>
+        <v>31.125</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>40.799999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1218,22 +1213,22 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>16.399999999999999</v>
+        <v>10.25</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>5.8</v>
+        <v>3.625</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>38.9</v>
+        <v>32.75</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1245,22 +1240,22 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>13.75</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>5.8</v>
+        <v>3.625</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>44.5</v>
+        <v>36.25</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1272,22 +1267,22 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>19.2</v>
+        <v>12</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>5.25</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>41.7</v>
+        <v>34.5</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1299,22 +1294,22 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>19.2</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>12.4</v>
+        <v>7.75</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>41.7</v>
+        <v>34.5</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1326,22 +1321,22 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>25.8</v>
+        <v>16.125</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>5.8</v>
+        <v>3.625</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>48.3</v>
+        <v>38.625</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1353,22 +1348,22 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>23.8</v>
+        <v>14.875</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="1"/>
-        <v>11.4</v>
+        <v>7.125</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>46.3</v>
+        <v>37.375</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1380,22 +1375,22 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>21.8</v>
+        <v>13.625</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>10.625</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>44.3</v>
+        <v>36.125</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1407,22 +1402,22 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>54.5</v>
+        <v>42.5</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1434,22 +1429,22 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>10.625</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>54.5</v>
+        <v>42.5</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1461,22 +1456,22 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>42.4</v>
+        <v>26.5</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
+        <v>22.375</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>64.900000000000006</v>
+        <v>49</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1488,22 +1483,22 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>41.6</v>
+        <v>26</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>16.875</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>64.099999999999994</v>
+        <v>48.5</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>25</v>
       </c>
@@ -1515,22 +1510,22 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>41.6</v>
+        <v>26</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
-        <v>18.2</v>
+        <v>11.375</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>64.099999999999994</v>
+        <v>48.5</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>26</v>
       </c>
@@ -1542,22 +1537,22 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>42.4</v>
+        <v>26.5</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
-        <v>9.4</v>
+        <v>5.875</v>
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>64.900000000000006</v>
+        <v>49</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1569,22 +1564,22 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>47.4</v>
+        <v>29.625</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="1"/>
-        <v>33.799999999999997</v>
+        <v>21.125</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>69.900000000000006</v>
+        <v>52.125</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>28</v>
       </c>
@@ -1596,22 +1591,22 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>29.25</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="1"/>
-        <v>26.4</v>
+        <v>16.5</v>
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>69.3</v>
+        <v>51.75</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>29</v>
       </c>
@@ -1623,22 +1618,22 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>29.25</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>11.75</v>
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>69.3</v>
+        <v>51.75</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>30</v>
       </c>
@@ -1650,22 +1645,22 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>47.4</v>
+        <v>29.625</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="1"/>
-        <v>11.4</v>
+        <v>7.125</v>
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>69.900000000000006</v>
+        <v>52.125</v>
       </c>
       <c r="J29">
         <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>31</v>
       </c>
@@ -1677,22 +1672,22 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>48.8</v>
+        <v>30.5</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>2.625</v>
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>71.3</v>
+        <v>53</v>
       </c>
       <c r="J30">
         <f t="shared" si="3"/>
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>32</v>
       </c>
@@ -1704,22 +1699,22 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>54.2</v>
+        <v>33.875</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>6.625</v>
       </c>
       <c r="I31">
         <f t="shared" si="2"/>
-        <v>76.7</v>
+        <v>56.375</v>
       </c>
       <c r="J31">
         <f t="shared" si="3"/>
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>33</v>
       </c>
@@ -1731,22 +1726,22 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>57.2</v>
+        <v>35.75</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="1"/>
-        <v>18.399999999999999</v>
+        <v>11.5</v>
       </c>
       <c r="I32">
         <f t="shared" si="2"/>
-        <v>79.7</v>
+        <v>58.25</v>
       </c>
       <c r="J32">
         <f t="shared" si="3"/>
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>34</v>
       </c>
@@ -1758,22 +1753,22 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>57.2</v>
+        <v>35.75</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="1"/>
-        <v>26.8</v>
+        <v>16.75</v>
       </c>
       <c r="I33">
         <f t="shared" si="2"/>
-        <v>79.7</v>
+        <v>58.25</v>
       </c>
       <c r="J33">
         <f t="shared" si="3"/>
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>35</v>
       </c>
@@ -1785,22 +1780,22 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>54.2</v>
+        <v>33.875</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="1"/>
-        <v>34.6</v>
+        <v>21.625</v>
       </c>
       <c r="I34">
         <f t="shared" si="2"/>
-        <v>76.7</v>
+        <v>56.375</v>
       </c>
       <c r="J34">
         <f t="shared" si="3"/>
-        <v>34.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21.625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>36</v>
       </c>
@@ -1812,22 +1807,22 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" si="0"/>
-        <v>48.8</v>
+        <v>30.5</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>25.625</v>
       </c>
       <c r="I35">
         <f t="shared" si="2"/>
-        <v>71.3</v>
+        <v>53</v>
       </c>
       <c r="J35">
         <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>25.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>37</v>
       </c>
@@ -1839,22 +1834,22 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" si="0"/>
-        <v>63.4</v>
+        <v>39.625</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="1"/>
-        <v>4.8</v>
+        <v>3</v>
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>85.9</v>
+        <v>62.125</v>
       </c>
       <c r="J36">
         <f t="shared" si="3"/>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>38</v>
       </c>
@@ -1866,22 +1861,22 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" si="0"/>
-        <v>63.4</v>
+        <v>39.625</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="1"/>
-        <v>10.4</v>
+        <v>6.5</v>
       </c>
       <c r="I37">
         <f t="shared" si="2"/>
-        <v>85.9</v>
+        <v>62.125</v>
       </c>
       <c r="J37">
         <f t="shared" si="3"/>
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>39</v>
       </c>
@@ -1893,22 +1888,22 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" si="0"/>
-        <v>63.4</v>
+        <v>39.625</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I38">
         <f t="shared" si="2"/>
-        <v>85.9</v>
+        <v>62.125</v>
       </c>
       <c r="J38">
         <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>40</v>
       </c>
@@ -1920,22 +1915,22 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="0"/>
-        <v>63.4</v>
+        <v>39.625</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="1"/>
-        <v>20.399999999999999</v>
+        <v>12.75</v>
       </c>
       <c r="I39">
         <f t="shared" si="2"/>
-        <v>85.9</v>
+        <v>62.125</v>
       </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>20.399999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>41</v>
       </c>
@@ -1947,22 +1942,22 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>44.375</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="1"/>
-        <v>3.4</v>
+        <v>2.125</v>
       </c>
       <c r="I40">
         <f t="shared" si="2"/>
-        <v>93.5</v>
+        <v>66.875</v>
       </c>
       <c r="J40">
         <f t="shared" si="3"/>
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>45</v>
       </c>
@@ -1974,22 +1969,22 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="0"/>
-        <v>67.2</v>
+        <v>42</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" si="1"/>
-        <v>3.4</v>
+        <v>2.125</v>
       </c>
       <c r="I41">
         <f t="shared" si="2"/>
-        <v>89.7</v>
+        <v>64.5</v>
       </c>
       <c r="J41">
         <f t="shared" si="3"/>
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>46</v>
       </c>
@@ -2001,22 +1996,22 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
-        <v>67.2</v>
+        <v>42</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="1"/>
-        <v>9.8000000000000007</v>
+        <v>6.125</v>
       </c>
       <c r="I42">
         <f t="shared" si="2"/>
-        <v>89.7</v>
+        <v>64.5</v>
       </c>
       <c r="J42">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>47</v>
       </c>
@@ -2028,22 +2023,22 @@
       </c>
       <c r="F43" s="1">
         <f t="shared" si="0"/>
-        <v>67.2</v>
+        <v>42</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I43">
         <f t="shared" si="2"/>
-        <v>89.7</v>
+        <v>64.5</v>
       </c>
       <c r="J43">
         <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>48</v>
       </c>
@@ -2055,22 +2050,22 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" si="0"/>
-        <v>67.2</v>
+        <v>42</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>13.75</v>
       </c>
       <c r="I44">
         <f t="shared" si="2"/>
-        <v>89.7</v>
+        <v>64.5</v>
       </c>
       <c r="J44">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>49</v>
       </c>
@@ -2082,22 +2077,22 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>44.375</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>13.75</v>
       </c>
       <c r="I45">
         <f t="shared" si="2"/>
-        <v>93.5</v>
+        <v>66.875</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>50</v>
       </c>
@@ -2109,22 +2104,22 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" si="0"/>
-        <v>77.400000000000006</v>
+        <v>48.375</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="1"/>
-        <v>12.8</v>
+        <v>8</v>
       </c>
       <c r="I46">
         <f t="shared" si="2"/>
-        <v>99.9</v>
+        <v>70.875</v>
       </c>
       <c r="J46">
         <f t="shared" si="3"/>
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>51</v>
       </c>
@@ -2136,22 +2131,22 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" si="0"/>
-        <v>77.400000000000006</v>
+        <v>48.375</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>10.625</v>
       </c>
       <c r="I47">
         <f t="shared" si="2"/>
-        <v>99.9</v>
+        <v>70.875</v>
       </c>
       <c r="J47">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>52</v>
       </c>
@@ -2163,22 +2158,22 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" si="0"/>
-        <v>87.8</v>
+        <v>54.875</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
+        <v>22.375</v>
       </c>
       <c r="I48">
         <f t="shared" si="2"/>
-        <v>110.3</v>
+        <v>77.375</v>
       </c>
       <c r="J48">
         <f t="shared" si="3"/>
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22.375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>53</v>
       </c>
@@ -2190,22 +2185,22 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>54.375</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>16.875</v>
       </c>
       <c r="I49">
         <f t="shared" si="2"/>
-        <v>109.5</v>
+        <v>76.875</v>
       </c>
       <c r="J49">
         <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.875</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>54</v>
       </c>
@@ -2217,22 +2212,22 @@
       </c>
       <c r="F50" s="1">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>54.375</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="1"/>
-        <v>18.2</v>
+        <v>11.375</v>
       </c>
       <c r="I50">
         <f t="shared" si="2"/>
-        <v>109.5</v>
+        <v>76.875</v>
       </c>
       <c r="J50">
         <f t="shared" si="3"/>
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>55</v>
       </c>
@@ -2244,22 +2239,22 @@
       </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
-        <v>87.8</v>
+        <v>54.875</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="1"/>
-        <v>9.4</v>
+        <v>5.875</v>
       </c>
       <c r="I51">
         <f t="shared" si="2"/>
-        <v>110.3</v>
+        <v>77.375</v>
       </c>
       <c r="J51">
         <f t="shared" si="3"/>
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.875</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>56</v>
       </c>
@@ -2271,22 +2266,22 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" si="0"/>
-        <v>92.8</v>
+        <v>58</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="1"/>
-        <v>33.799999999999997</v>
+        <v>21.125</v>
       </c>
       <c r="I52">
         <f t="shared" si="2"/>
-        <v>115.3</v>
+        <v>80.5</v>
       </c>
       <c r="J52">
         <f t="shared" si="3"/>
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>57</v>
       </c>
@@ -2298,22 +2293,22 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" si="0"/>
-        <v>92.2</v>
+        <v>57.625</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="1"/>
-        <v>26.4</v>
+        <v>16.5</v>
       </c>
       <c r="I53">
         <f t="shared" si="2"/>
-        <v>114.7</v>
+        <v>80.125</v>
       </c>
       <c r="J53">
         <f t="shared" si="3"/>
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>58</v>
       </c>
@@ -2325,22 +2320,22 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" si="0"/>
-        <v>92.2</v>
+        <v>57.625</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="1"/>
-        <v>18.8</v>
+        <v>11.75</v>
       </c>
       <c r="I54">
         <f t="shared" si="2"/>
-        <v>114.7</v>
+        <v>80.125</v>
       </c>
       <c r="J54">
         <f t="shared" si="3"/>
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>59</v>
       </c>
@@ -2352,22 +2347,22 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" si="0"/>
-        <v>92.8</v>
+        <v>58</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="1"/>
-        <v>11.4</v>
+        <v>7.125</v>
       </c>
       <c r="I55">
         <f t="shared" si="2"/>
-        <v>115.3</v>
+        <v>80.5</v>
       </c>
       <c r="J55">
         <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>65</v>
       </c>
@@ -2379,22 +2374,22 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" si="0"/>
-        <v>94.2</v>
+        <v>58.875</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>2.625</v>
       </c>
       <c r="I56">
         <f t="shared" si="2"/>
-        <v>116.7</v>
+        <v>81.375</v>
       </c>
       <c r="J56">
         <f t="shared" si="3"/>
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>66</v>
       </c>
@@ -2406,22 +2401,22 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="0"/>
-        <v>99.6</v>
+        <v>62.25</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="1"/>
-        <v>10.6</v>
+        <v>6.625</v>
       </c>
       <c r="I57">
         <f t="shared" si="2"/>
-        <v>122.1</v>
+        <v>84.75</v>
       </c>
       <c r="J57">
         <f t="shared" si="3"/>
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>67</v>
       </c>
@@ -2433,22 +2428,22 @@
       </c>
       <c r="F58" s="1">
         <f t="shared" si="0"/>
-        <v>102.6</v>
+        <v>64.125</v>
       </c>
       <c r="G58" s="1">
         <f t="shared" si="1"/>
-        <v>18.399999999999999</v>
+        <v>11.5</v>
       </c>
       <c r="I58">
         <f t="shared" si="2"/>
-        <v>125.1</v>
+        <v>86.625</v>
       </c>
       <c r="J58">
         <f t="shared" si="3"/>
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>68</v>
       </c>
@@ -2460,22 +2455,22 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" si="0"/>
-        <v>102.6</v>
+        <v>64.125</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" si="1"/>
-        <v>26.8</v>
+        <v>16.75</v>
       </c>
       <c r="I59">
         <f t="shared" si="2"/>
-        <v>125.1</v>
+        <v>86.625</v>
       </c>
       <c r="J59">
         <f t="shared" si="3"/>
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>69</v>
       </c>
@@ -2487,22 +2482,22 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" si="0"/>
-        <v>99.6</v>
+        <v>62.25</v>
       </c>
       <c r="G60" s="1">
         <f t="shared" si="1"/>
-        <v>34.6</v>
+        <v>21.625</v>
       </c>
       <c r="I60">
         <f t="shared" si="2"/>
-        <v>122.1</v>
+        <v>84.75</v>
       </c>
       <c r="J60">
         <f t="shared" si="3"/>
-        <v>34.6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21.625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>70</v>
       </c>
@@ -2514,22 +2509,22 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" si="0"/>
-        <v>94.2</v>
+        <v>58.875</v>
       </c>
       <c r="G61" s="1">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>25.625</v>
       </c>
       <c r="I61">
         <f t="shared" si="2"/>
-        <v>116.7</v>
+        <v>81.375</v>
       </c>
       <c r="J61">
         <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>25.625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>71</v>
       </c>
@@ -2541,22 +2536,22 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" si="0"/>
-        <v>107.4</v>
+        <v>67.125</v>
       </c>
       <c r="G62" s="1">
         <f t="shared" si="1"/>
-        <v>19.600000000000001</v>
+        <v>12.25</v>
       </c>
       <c r="I62">
         <f t="shared" si="2"/>
-        <v>129.9</v>
+        <v>89.625</v>
       </c>
       <c r="J62">
         <f t="shared" si="3"/>
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>72</v>
       </c>
@@ -2568,22 +2563,22 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" si="0"/>
-        <v>107.4</v>
+        <v>67.125</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>7.625</v>
       </c>
       <c r="I63">
         <f t="shared" si="2"/>
-        <v>129.9</v>
+        <v>89.625</v>
       </c>
       <c r="J63">
         <f t="shared" si="3"/>
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>73</v>
       </c>
@@ -2595,22 +2590,22 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>67.5</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="I64">
         <f t="shared" si="2"/>
-        <v>130.5</v>
+        <v>90</v>
       </c>
       <c r="J64">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>74</v>
       </c>
@@ -2622,22 +2617,22 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" si="0"/>
-        <v>112.4</v>
+        <v>70.25</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" si="1"/>
-        <v>3.6</v>
+        <v>2.25</v>
       </c>
       <c r="I65">
         <f t="shared" si="2"/>
-        <v>134.9</v>
+        <v>92.75</v>
       </c>
       <c r="J65">
         <f t="shared" si="3"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>75</v>
       </c>
@@ -2649,22 +2644,22 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ref="F66:F82" si="4">(B66*1000)/$M$1</f>
-        <v>116.8</v>
+        <v>73</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" ref="G66:G82" si="5">(C66*1000)/$M$1</f>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I83" si="6">(F66+$M$4)*$M$2</f>
-        <v>139.30000000000001</v>
+        <f t="shared" ref="I66:I82" si="6">(F66*$M$2)+$M$4</f>
+        <v>95.5</v>
       </c>
       <c r="J66">
-        <f t="shared" ref="J66:J83" si="7">(G66+$M$5)*$M$3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J66:J82" si="7">(G66*$M$3)+$M$5</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>76</v>
       </c>
@@ -2676,22 +2671,22 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" si="4"/>
-        <v>117.4</v>
+        <v>73.375</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" si="5"/>
-        <v>12.2</v>
+        <v>7.625</v>
       </c>
       <c r="I67">
         <f t="shared" si="6"/>
-        <v>139.9</v>
+        <v>95.875</v>
       </c>
       <c r="J67">
         <f t="shared" si="7"/>
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>80</v>
       </c>
@@ -2703,22 +2698,22 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" si="4"/>
-        <v>117.4</v>
+        <v>73.375</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="5"/>
-        <v>19.600000000000001</v>
+        <v>12.25</v>
       </c>
       <c r="I68">
         <f t="shared" si="6"/>
-        <v>139.9</v>
+        <v>95.875</v>
       </c>
       <c r="J68">
         <f t="shared" si="7"/>
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>81</v>
       </c>
@@ -2730,22 +2725,22 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" si="4"/>
-        <v>110.8</v>
+        <v>69.25</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>5.625</v>
       </c>
       <c r="I69">
         <f t="shared" si="6"/>
-        <v>133.30000000000001</v>
+        <v>91.75</v>
       </c>
       <c r="J69">
         <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>82</v>
       </c>
@@ -2757,22 +2752,22 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="4"/>
-        <v>110.8</v>
+        <v>69.25</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" si="5"/>
-        <v>14.8</v>
+        <v>9.25</v>
       </c>
       <c r="I70">
         <f t="shared" si="6"/>
-        <v>133.30000000000001</v>
+        <v>91.75</v>
       </c>
       <c r="J70">
         <f t="shared" si="7"/>
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>83</v>
       </c>
@@ -2784,22 +2779,22 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" si="4"/>
-        <v>110.8</v>
+        <v>69.25</v>
       </c>
       <c r="G71" s="1">
         <f t="shared" si="5"/>
-        <v>20.6</v>
+        <v>12.875</v>
       </c>
       <c r="I71">
         <f t="shared" si="6"/>
-        <v>133.30000000000001</v>
+        <v>91.75</v>
       </c>
       <c r="J71">
         <f t="shared" si="7"/>
-        <v>20.6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>84</v>
       </c>
@@ -2811,22 +2806,22 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" si="4"/>
-        <v>123.4</v>
+        <v>77.125</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" si="5"/>
-        <v>12.4</v>
+        <v>7.75</v>
       </c>
       <c r="I72">
         <f t="shared" si="6"/>
-        <v>145.9</v>
+        <v>99.625</v>
       </c>
       <c r="J72">
         <f t="shared" si="7"/>
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>85</v>
       </c>
@@ -2838,22 +2833,22 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" si="4"/>
-        <v>123.2</v>
+        <v>77</v>
       </c>
       <c r="G73" s="1">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>11.875</v>
       </c>
       <c r="I73">
         <f t="shared" si="6"/>
-        <v>145.69999999999999</v>
+        <v>99.5</v>
       </c>
       <c r="J73">
         <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>86</v>
       </c>
@@ -2865,22 +2860,22 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" si="4"/>
-        <v>122.8</v>
+        <v>76.75</v>
       </c>
       <c r="G74" s="1">
         <f t="shared" si="5"/>
-        <v>25.6</v>
+        <v>16</v>
       </c>
       <c r="I74">
         <f t="shared" si="6"/>
-        <v>145.30000000000001</v>
+        <v>99.25</v>
       </c>
       <c r="J74">
         <f t="shared" si="7"/>
-        <v>25.6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>87</v>
       </c>
@@ -2892,22 +2887,22 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" si="4"/>
-        <v>122.6</v>
+        <v>76.625</v>
       </c>
       <c r="G75" s="1">
         <f t="shared" si="5"/>
-        <v>32.200000000000003</v>
+        <v>20.125</v>
       </c>
       <c r="I75">
         <f t="shared" si="6"/>
-        <v>145.1</v>
+        <v>99.125</v>
       </c>
       <c r="J75">
         <f t="shared" si="7"/>
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20.125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>88</v>
       </c>
@@ -2919,22 +2914,22 @@
       </c>
       <c r="F76" s="1">
         <f t="shared" si="4"/>
-        <v>122.4</v>
+        <v>76.5</v>
       </c>
       <c r="G76" s="1">
         <f t="shared" si="5"/>
-        <v>38.799999999999997</v>
+        <v>24.25</v>
       </c>
       <c r="I76">
         <f t="shared" si="6"/>
-        <v>144.9</v>
+        <v>99</v>
       </c>
       <c r="J76">
         <f t="shared" si="7"/>
-        <v>38.799999999999997</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>89</v>
       </c>
@@ -2946,22 +2941,22 @@
       </c>
       <c r="F77" s="1">
         <f t="shared" si="4"/>
-        <v>126.4</v>
+        <v>79</v>
       </c>
       <c r="G77" s="1">
         <f t="shared" si="5"/>
-        <v>12.4</v>
+        <v>7.75</v>
       </c>
       <c r="I77">
         <f t="shared" si="6"/>
-        <v>148.9</v>
+        <v>101.5</v>
       </c>
       <c r="J77">
         <f t="shared" si="7"/>
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>90</v>
       </c>
@@ -2973,22 +2968,22 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" si="4"/>
-        <v>126.4</v>
+        <v>79</v>
       </c>
       <c r="G78" s="1">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>11.875</v>
       </c>
       <c r="I78">
         <f t="shared" si="6"/>
-        <v>148.9</v>
+        <v>101.5</v>
       </c>
       <c r="J78">
         <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>91</v>
       </c>
@@ -3000,22 +2995,22 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" si="4"/>
-        <v>126.6</v>
+        <v>79.125</v>
       </c>
       <c r="G79" s="1">
         <f t="shared" si="5"/>
-        <v>25.6</v>
+        <v>16</v>
       </c>
       <c r="I79">
         <f t="shared" si="6"/>
-        <v>149.1</v>
+        <v>101.625</v>
       </c>
       <c r="J79">
         <f t="shared" si="7"/>
-        <v>25.6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>92</v>
       </c>
@@ -3027,22 +3022,22 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" si="4"/>
-        <v>126.6</v>
+        <v>79.125</v>
       </c>
       <c r="G80" s="1">
         <f t="shared" si="5"/>
-        <v>32.200000000000003</v>
+        <v>20.125</v>
       </c>
       <c r="I80">
         <f t="shared" si="6"/>
-        <v>149.1</v>
+        <v>101.625</v>
       </c>
       <c r="J80">
         <f t="shared" si="7"/>
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20.125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>93</v>
       </c>
@@ -3054,22 +3049,22 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" si="4"/>
-        <v>126.6</v>
+        <v>79.125</v>
       </c>
       <c r="G81" s="1">
         <f t="shared" si="5"/>
-        <v>38.799999999999997</v>
+        <v>24.25</v>
       </c>
       <c r="I81">
         <f t="shared" si="6"/>
-        <v>149.1</v>
+        <v>101.625</v>
       </c>
       <c r="J81">
         <f t="shared" si="7"/>
-        <v>38.799999999999997</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24.25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>94</v>
       </c>
@@ -3081,74 +3076,74 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>78.125</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" si="5"/>
-        <v>5.2</v>
+        <v>3.25</v>
       </c>
       <c r="I82">
         <f t="shared" si="6"/>
-        <v>147.5</v>
+        <v>100.625</v>
       </c>
       <c r="J82">
         <f t="shared" si="7"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="B83"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="B84"/>
       <c r="C84"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="B85"/>
       <c r="C85"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="B86"/>
       <c r="C86"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="B87"/>
       <c r="C87"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="B88"/>
       <c r="C88"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="B89"/>
       <c r="C89"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="B90"/>
       <c r="C90"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="B91"/>
       <c r="C91"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="B92"/>
       <c r="C92"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="B93"/>
       <c r="C93"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="B94"/>
       <c r="C94"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="B95"/>
       <c r="C95"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="B96"/>
       <c r="C96"/>
     </row>

</xml_diff>